<commit_message>
Added support for wildcard cases
</commit_message>
<xml_diff>
--- a/test_files/tokenization/wildcards.xlsx
+++ b/test_files/tokenization/wildcards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brt.hawayda\Desktop\42\minishell\minishell-tester\test_files\tokenization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554FF281-A4EE-4B3A-B1B7-DB16169C6422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDC1E84-A409-44C1-9F37-18AFDB53EAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,181 +27,181 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
-    <t>$&gt; *.c</t>
-  </si>
-  <si>
-    <t>$&gt; ?.md</t>
-  </si>
-  <si>
-    <t>$&gt; images_??.png</t>
-  </si>
-  <si>
-    <t>$&gt; file[0-9].log</t>
-  </si>
-  <si>
-    <t>$&gt; file[01][0-9].log</t>
-  </si>
-  <si>
-    <t>$&gt; *.?sv</t>
-  </si>
-  <si>
-    <t>$&gt; data_*_202[0-9].csv</t>
-  </si>
-  <si>
-    <t>$&gt; report-??-*.pdf</t>
-  </si>
-  <si>
-    <t>$&gt; log_[a-z][a-z].txt</t>
-  </si>
-  <si>
-    <t>$&gt; *.[ch]</t>
-  </si>
-  <si>
-    <t>$&gt; module[1-9]*.cpp</t>
-  </si>
-  <si>
-    <t>$&gt; backup-*[!aeiou].tar</t>
-  </si>
-  <si>
-    <t>$&gt; ??_summary_*.docx</t>
-  </si>
-  <si>
-    <t>$&gt; config?[0-9]?.ini</t>
-  </si>
-  <si>
-    <t>$&gt; test_*_v[1-9].*</t>
-  </si>
-  <si>
-    <t>$&gt; *_report_[A-Z][A-Z].csv</t>
-  </si>
-  <si>
-    <t>$&gt; data[0-3]?_error.log</t>
-  </si>
-  <si>
-    <t>$&gt; *_v[0-9].[0-9].[0-9].bin</t>
-  </si>
-  <si>
-    <t>$&gt; shell_???.sh</t>
-  </si>
-  <si>
-    <t>$&gt; user*-ctrl?.dat</t>
-  </si>
-  <si>
-    <t>$&gt; arch[abc]ive.zip</t>
-  </si>
-  <si>
-    <t>$&gt; *-*-*-backup.*</t>
-  </si>
-  <si>
-    <t>$&gt; notes_20[12][0-9].txt</t>
-  </si>
-  <si>
-    <t>$&gt; session??.log</t>
-  </si>
-  <si>
-    <t>$&gt; log-202[0-9]-[01][0-9]-*.log</t>
-  </si>
-  <si>
-    <t>$&gt; file*[0-9]?.[ch]</t>
-  </si>
-  <si>
-    <t>$&gt; data??_backup_*.tar.gz</t>
-  </si>
-  <si>
-    <t>$&gt; [!abc]*[xyz]?.txt</t>
-  </si>
-  <si>
-    <t>$&gt; prefix*mid?fix*suffix.log</t>
-  </si>
-  <si>
-    <t>$&gt; *[^aeiou]*.[ch]</t>
-  </si>
-  <si>
-    <t>$&gt; report_[0-9][0-9][0-9]?.csv</t>
-  </si>
-  <si>
-    <t>$&gt; .*hidden*[!0-9].dat</t>
-  </si>
-  <si>
-    <t>$&gt; ?start*end?</t>
-  </si>
-  <si>
-    <t>$&gt; even*more*complex?pattern[0-9].log</t>
-  </si>
-  <si>
-    <t>$&gt; multi[0-9][!5-7]?*[a-z].data</t>
-  </si>
-  <si>
-    <t>$&gt; *error??[!0-9]*.log</t>
-  </si>
-  <si>
-    <t>$&gt; [!a-zA-Z]?*-data[!8-9]?.[^ch]</t>
-  </si>
-  <si>
-    <t>$&gt; project_[0-9][0-9]_release?_[!x-z].tar.gz</t>
-  </si>
-  <si>
-    <t>$&gt; nested*pattern*with?many[0-9]parts[abc].dat</t>
-  </si>
-  <si>
-    <t>$&gt; *[!0-9?]*[a-z][!A-Z]?*.ext</t>
-  </si>
-  <si>
-    <t>$&gt; customer_[A-Za-z]*??[0-9].backup.tar</t>
-  </si>
-  <si>
-    <t>$&gt; log-*-week[1-4]-[!5-9]?report?.txt</t>
-  </si>
-  <si>
-    <t>$&gt; [abc][!abc]*??[a-c]?x[!z].cfg</t>
-  </si>
-  <si>
-    <t>$&gt; *.[ch]?_*.[ch]?</t>
-  </si>
-  <si>
-    <t>$&gt; prefix[0-9]*suffix?[!xyz][a-c].log</t>
-  </si>
-  <si>
-    <t>$&gt; backup_[!ab]*[0-9]?_*.[!aeiou]?z.bak</t>
-  </si>
-  <si>
-    <t>$&gt; alpha?*[0-9][A-F]??.hex</t>
-  </si>
-  <si>
-    <t>$&gt; ??*[*]literal?*.tmp</t>
-  </si>
-  <si>
-    <t>$&gt; abc*xyz*123??[5-7].bin</t>
-  </si>
-  <si>
-    <t>$&gt; [!0-9][0-9]?*file[!G-M].data</t>
-  </si>
-  <si>
-    <t>$&gt; long*pattern?with*many?stars*[abc]?end.log</t>
-  </si>
-  <si>
-    <t>$&gt; *multi?level*test[1-3]?case[!x].out</t>
-  </si>
-  <si>
-    <t>$&gt; start?middle*s?t[!ae]nd.gz</t>
-  </si>
-  <si>
-    <t>$&gt; data[2-4][A-C]?file*202[0-3].xlsx</t>
-  </si>
-  <si>
-    <t>$&gt; *_?[*][!x-z]*?.doc</t>
-  </si>
-  <si>
-    <t>$&gt; [?*]*file[*?].txt</t>
-  </si>
-  <si>
-    <t>$&gt; *.[ch][!hp]*.orig</t>
-  </si>
-  <si>
-    <t>$&gt; file[0-9]?_*[a-z][!m-p].data</t>
-  </si>
-  <si>
-    <t>$&gt; session[0-9][0-9]?_*[A-Z]?final.*</t>
+    <t>$&gt; *</t>
+  </si>
+  <si>
+    <t>$&gt; **</t>
+  </si>
+  <si>
+    <t>$&gt; images_*</t>
+  </si>
+  <si>
+    <t>$&gt; file[0-9]</t>
+  </si>
+  <si>
+    <t>$&gt; file[01][0-9]</t>
+  </si>
+  <si>
+    <t>$&gt; *sv</t>
+  </si>
+  <si>
+    <t>$&gt; data_*_202[0-9]</t>
+  </si>
+  <si>
+    <t>$&gt; report-*-*</t>
+  </si>
+  <si>
+    <t>$&gt; log_[a-z][a-z]</t>
+  </si>
+  <si>
+    <t>$&gt; *ch]</t>
+  </si>
+  <si>
+    <t>$&gt; module[1-9]*</t>
+  </si>
+  <si>
+    <t>$&gt; backup-*[!aeiou]</t>
+  </si>
+  <si>
+    <t>$&gt; *_summary_*</t>
+  </si>
+  <si>
+    <t>$&gt; config*[0-9]*</t>
+  </si>
+  <si>
+    <t>$&gt; test_*_v[1-9]</t>
+  </si>
+  <si>
+    <t>$&gt; *_report_[A-Z][A-Z]</t>
+  </si>
+  <si>
+    <t>$&gt; data[0-3]*_error</t>
+  </si>
+  <si>
+    <t>$&gt; *_v[0-9]0-9]0-9]</t>
+  </si>
+  <si>
+    <t>$&gt; shell_*</t>
+  </si>
+  <si>
+    <t>$&gt; user*-ctrl*</t>
+  </si>
+  <si>
+    <t>$&gt; arch[abc]ive</t>
+  </si>
+  <si>
+    <t>$&gt; *-*-*-backup</t>
+  </si>
+  <si>
+    <t>$&gt; notes_20[12][0-9]</t>
+  </si>
+  <si>
+    <t>$&gt; session*</t>
+  </si>
+  <si>
+    <t>$&gt; log-202[0-9]-[01][0-9]-*</t>
+  </si>
+  <si>
+    <t>$&gt; file*[0-9]*ch]</t>
+  </si>
+  <si>
+    <t>$&gt; data*_backup_*</t>
+  </si>
+  <si>
+    <t>$&gt; [!abc]*[xyz]*</t>
+  </si>
+  <si>
+    <t>$&gt; prefix*mid*fix*suffix</t>
+  </si>
+  <si>
+    <t>$&gt; *[^aeiou]*ch]</t>
+  </si>
+  <si>
+    <t>$&gt; report_[0-9][0-9][0-9]*</t>
+  </si>
+  <si>
+    <t>$&gt; hidden*[!0-9]</t>
+  </si>
+  <si>
+    <t>$&gt; *start*end*</t>
+  </si>
+  <si>
+    <t>$&gt; even*more*complex*pattern[0-9]</t>
+  </si>
+  <si>
+    <t>$&gt; multi[0-9][!5-7]**[a-z]</t>
+  </si>
+  <si>
+    <t>$&gt; *error*[!0-9]*</t>
+  </si>
+  <si>
+    <t>$&gt; [!a-zA-Z]**-data[!8-9]*ch]</t>
+  </si>
+  <si>
+    <t>$&gt; project_[0-9][0-9]_release*_[!x-z]</t>
+  </si>
+  <si>
+    <t>$&gt; nested*pattern*with*many[0-9]parts[abc]</t>
+  </si>
+  <si>
+    <t>$&gt; *[!0-9*]*[a-z][!A-Z]**</t>
+  </si>
+  <si>
+    <t>$&gt; customer_[A-Za-z]**[0-9]</t>
+  </si>
+  <si>
+    <t>$&gt; log-*-week[1-4]-[!5-9]*report*</t>
+  </si>
+  <si>
+    <t>$&gt; [abc][!abc]**[a-c]*x[!z]</t>
+  </si>
+  <si>
+    <t>$&gt; *ch]*_*ch]*</t>
+  </si>
+  <si>
+    <t>$&gt; prefix[0-9]*suffix*[!xyz][a-c]</t>
+  </si>
+  <si>
+    <t>$&gt; backup_[!ab]*[0-9]*_*aeiou]*z</t>
+  </si>
+  <si>
+    <t>$&gt; alpha**[0-9][A-F]*</t>
+  </si>
+  <si>
+    <t>$&gt; **[*]literal**</t>
+  </si>
+  <si>
+    <t>$&gt; abc*xyz*123*[5-7]</t>
+  </si>
+  <si>
+    <t>$&gt; [!0-9][0-9]**file[!G-M]</t>
+  </si>
+  <si>
+    <t>$&gt; long*pattern*with*many*stars*[abc]*end</t>
+  </si>
+  <si>
+    <t>$&gt; *multi*level*test[1-3]*case[!x]</t>
+  </si>
+  <si>
+    <t>$&gt; start*middle*s*t[!ae]nd</t>
+  </si>
+  <si>
+    <t>$&gt; data[2-4][A-C]*file*202[0-3]</t>
+  </si>
+  <si>
+    <t>$&gt; *_*[*][!x-z]**</t>
+  </si>
+  <si>
+    <t>$&gt; [**]*file[**]</t>
+  </si>
+  <si>
+    <t>$&gt; *ch][!hp]*</t>
+  </si>
+  <si>
+    <t>$&gt; file[0-9]*_*[a-z][!m-p]</t>
+  </si>
+  <si>
+    <t>$&gt; session[0-9][0-9]*_*[A-Z]*final</t>
   </si>
 </sst>
 </file>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A60" sqref="A1:A60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>